<commit_message>
Added messages for OpenAPI checks
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE3ADBC-C492-4C11-AA1E-23103394D70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B25DE04-9F0E-4302-870B-DA647AB4DA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51195" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="1" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="145">
   <si>
     <t>Class-Info</t>
   </si>
@@ -400,136 +400,316 @@
     <t>When working with OpenAPI and REST there are some restrictions concerning the data types that can be used in Java. This warning tells you that in a defined "BeanParam" at least one property uses an incompatible type. This will lead to an invalid request / response from an OpenAPI perspective.</t>
   </si>
   <si>
-    <t>&lt;&lt;BeanParam&gt;&gt; ''{0}'' has propertie(s) ''{1}'' that are not comaptible with OpenAPI (''{2}''). For further details please refer to FAQ entry #2.2 on https://anaptecs.atlassian.net/l/cp/ndmtZxvX</t>
-  </si>
-  <si>
-    <t>&lt;&lt;RESTOperation&gt;&gt; ''{0}(...)'' has parameter type(s) ''{1}'' that are not compatible with OpenAPI (''{2}''). For further details please refer to FAQ entry #2.2 on https://anaptecs.atlassian.net/l/cp/ndmtZxvX"</t>
-  </si>
-  <si>
     <t>'{0}'' seems to use file system references. This might lead to portabilty issues with the exported XMI files. For further details please refer to FAQ entry #2.1 on https://anaptecs.atlassian.net/l/cp/ndmtZxvX"</t>
   </si>
   <si>
     <t>com.anaptecs.jeaf.generator</t>
   </si>
   <si>
+    <t>STYLESHEET_NOT_AVAILABLE</t>
+  </si>
+  <si>
+    <t>UNABLE_TO_CREATE_DIR</t>
+  </si>
+  <si>
+    <t>UNABLE_TO_PERFORM_TRANSFORMATION</t>
+  </si>
+  <si>
+    <t>INVALID_CLASS_INFO</t>
+  </si>
+  <si>
+    <t>UNABLE_TO_OPEN_EXCEL_WORKBOOK</t>
+  </si>
+  <si>
+    <t>UNABLE_TO_CLOSE_EXCEL_WORKBOOK</t>
+  </si>
+  <si>
+    <t>CLASS_INFO_SHEET_MISSING</t>
+  </si>
+  <si>
+    <t>UNABLE_TO_CREATE_XML_DOCUMENT</t>
+  </si>
+  <si>
+    <t>NO_MESSAGE_DATA_IN_WORKBOOK</t>
+  </si>
+  <si>
+    <t>INVALID_MESSAGE_DATA</t>
+  </si>
+  <si>
+    <t>IGNORING_ROW</t>
+  </si>
+  <si>
+    <t>MESSAGE_ID_NOT_UNIQUE</t>
+  </si>
+  <si>
+    <t>MESSAGE_NAME_NOT_UNIQUE</t>
+  </si>
+  <si>
+    <t>IGNORING_EMPTY_SHEET</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if the style sheet that defines the transformation of the XML document containing error messages is not located within the applications class path.</t>
+  </si>
+  <si>
+    <t>XSLT style sheet ''{0}'' can not be found within the applications class path.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if the generator can not create an output directory for a generated class.</t>
+  </si>
+  <si>
+    <t>Unable to create directory ''{0}''.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if an exception occurs during the generation of the Java class using XSLT.</t>
+  </si>
+  <si>
+    <t>Unable to generate Java class ''{0}'' out of message resource ''{1}''.</t>
+  </si>
+  <si>
+    <t>Unable to convert Excel workbook to message resource file. Class-Information is incomplete or invalid. Affected field ''{0}'' in file ''{1}''.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown when an exception occurs when trying to open an Excel workbook.</t>
+  </si>
+  <si>
+    <t>Unable to open Excel workbook ''{0}''. {1}</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown when an exception occurs when trying to close an Excel workbook.</t>
+  </si>
+  <si>
+    <t>Unable to close Excel workbook ''{0}''. {1}</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if class info is missing in the provided Excel workbook.</t>
+  </si>
+  <si>
+    <t>Required sheet ''{0}'' inside Excel workbook ''{1}'' is missing. Please ensure that you use the right Excel template for message resources.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if a new XML document could not be created.</t>
+  </si>
+  <si>
+    <t>Unable to create new XML document.</t>
+  </si>
+  <si>
+    <t>Excel workbook ''{0}'' does not contain any message data. Please ensure that the excel file contains at least one sheet with message data.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if a required column in message data is missing.</t>
+  </si>
+  <si>
+    <t>Excel sheet ''{0}'' does not contain required column with name ''{1}''. Please ensure that you use the right Excel template for message resources.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if values for one or more required fields are missing.</t>
+  </si>
+  <si>
+    <t>Ignoring row ''{1}'' in Excel sheet ''{0}'' as it does not contain values for all required columns. The following fields are missing: {2}</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if a message ID is used multiple times.</t>
+  </si>
+  <si>
+    <t>Message-ID ''{0}'' is not unique. Excel sheet ''{1}'' contains this message ID even though it was already used before. Please ensure that every message ID is globally only used once.</t>
+  </si>
+  <si>
+    <t>Exceptions with this error code are thrown if a message name is used multiple times.</t>
+  </si>
+  <si>
+    <t>Message-Name ''{0}'' is not unique. Excel sheet ''{1}'' contains this name even though it was already used before. Please ensure that every message name is only used once per Excel file.</t>
+  </si>
+  <si>
+    <t>Ignoring empty sheet ''{0}'' within Excel workbook.</t>
+  </si>
+  <si>
+    <t>INVALID_REST_RESOURCE_PATH</t>
+  </si>
+  <si>
+    <t>When defining the path of a REST resource then the path that is defined on the RESTResource (not RESTOperation) must start with a '/'</t>
+  </si>
+  <si>
     <t>JEAF Generator expects JEAF Meta Model (JMM) revision ''{0}'' or higher. Please update your UML project to a newer version of JMM. Your current revision is: {1}</t>
   </si>
   <si>
-    <t>STYLESHEET_NOT_AVAILABLE</t>
-  </si>
-  <si>
-    <t>UNABLE_TO_CREATE_DIR</t>
-  </si>
-  <si>
-    <t>UNABLE_TO_PERFORM_TRANSFORMATION</t>
-  </si>
-  <si>
-    <t>INVALID_CLASS_INFO</t>
-  </si>
-  <si>
-    <t>UNABLE_TO_OPEN_EXCEL_WORKBOOK</t>
-  </si>
-  <si>
-    <t>UNABLE_TO_CLOSE_EXCEL_WORKBOOK</t>
-  </si>
-  <si>
-    <t>CLASS_INFO_SHEET_MISSING</t>
-  </si>
-  <si>
-    <t>UNABLE_TO_CREATE_XML_DOCUMENT</t>
-  </si>
-  <si>
-    <t>NO_MESSAGE_DATA_IN_WORKBOOK</t>
-  </si>
-  <si>
-    <t>INVALID_MESSAGE_DATA</t>
-  </si>
-  <si>
-    <t>IGNORING_ROW</t>
-  </si>
-  <si>
-    <t>MESSAGE_ID_NOT_UNIQUE</t>
-  </si>
-  <si>
-    <t>MESSAGE_NAME_NOT_UNIQUE</t>
-  </si>
-  <si>
-    <t>IGNORING_EMPTY_SHEET</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if the style sheet that defines the transformation of the XML document containing error messages is not located within the applications class path.</t>
-  </si>
-  <si>
-    <t>XSLT style sheet ''{0}'' can not be found within the applications class path.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if the generator can not create an output directory for a generated class.</t>
-  </si>
-  <si>
-    <t>Unable to create directory ''{0}''.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if an exception occurs during the generation of the Java class using XSLT.</t>
-  </si>
-  <si>
-    <t>Unable to generate Java class ''{0}'' out of message resource ''{1}''.</t>
-  </si>
-  <si>
-    <t>Unable to convert Excel workbook to message resource file. Class-Information is incomplete or invalid. Affected field ''{0}'' in file ''{1}''.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown when an exception occurs when trying to open an Excel workbook.</t>
-  </si>
-  <si>
-    <t>Unable to open Excel workbook ''{0}''. {1}</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown when an exception occurs when trying to close an Excel workbook.</t>
-  </si>
-  <si>
-    <t>Unable to close Excel workbook ''{0}''. {1}</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if class info is missing in the provided Excel workbook.</t>
-  </si>
-  <si>
-    <t>Required sheet ''{0}'' inside Excel workbook ''{1}'' is missing. Please ensure that you use the right Excel template for message resources.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if a new XML document could not be created.</t>
-  </si>
-  <si>
-    <t>Unable to create new XML document.</t>
-  </si>
-  <si>
-    <t>Excel workbook ''{0}'' does not contain any message data. Please ensure that the excel file contains at least one sheet with message data.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if a required column in message data is missing.</t>
-  </si>
-  <si>
-    <t>Excel sheet ''{0}'' does not contain required column with name ''{1}''. Please ensure that you use the right Excel template for message resources.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if values for one or more required fields are missing.</t>
-  </si>
-  <si>
-    <t>Ignoring row ''{1}'' in Excel sheet ''{0}'' as it does not contain values for all required columns. The following fields are missing: {2}</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if a message ID is used multiple times.</t>
-  </si>
-  <si>
-    <t>Message-ID ''{0}'' is not unique. Excel sheet ''{1}'' contains this message ID even though it was already used before. Please ensure that every message ID is globally only used once.</t>
-  </si>
-  <si>
-    <t>Exceptions with this error code are thrown if a message name is used multiple times.</t>
-  </si>
-  <si>
-    <t>Message-Name ''{0}'' is not unique. Excel sheet ''{1}'' contains this name even though it was already used before. Please ensure that every message name is only used once per Excel file.</t>
-  </si>
-  <si>
-    <t>Ignoring empty sheet ''{0}'' within Excel workbook.</t>
+    <t>«RESTOperation» ''{0}(...)'' has parameter type(s) ''{1}'' that are not compatible with OpenAPI (''{2}''). For further details please refer to FAQ entry #2.2 on https://anaptecs.atlassian.net/l/cp/ndmtZxvX"</t>
+  </si>
+  <si>
+    <t>«BeanParam» ''{0}'' has propertie(s) ''{1}'' that are not comaptible with OpenAPI (''{2}''). For further details please refer to FAQ entry #2.2 on https://anaptecs.atlassian.net/l/cp/ndmtZxvX</t>
+  </si>
+  <si>
+    <t>The resource path of an "RESTOperation" is the combination of the path of the "RESTResource" and the "RESTOperation". However at least one of them has to be defined.</t>
+  </si>
+  <si>
+    <t>NO_REST_RESOURCE_PATH</t>
+  </si>
+  <si>
+    <t>INVALID_REST_OPERSTION_PATH</t>
+  </si>
+  <si>
+    <t>The path of a "RESTOperation" must not start with '/'.</t>
+  </si>
+  <si>
+    <t>Either «RESTResource» or «RESTOperation» must define a resource path for operation ''{0}(...)''</t>
+  </si>
+  <si>
+    <t>«RESTOperation» ''{0}(...)'' has an invalid path. Path of operation must not start with ''/''.</t>
+  </si>
+  <si>
+    <t>Resource path of «RESTResource» ''{0}'' must either start with ''/'' or might be not set at all.</t>
+  </si>
+  <si>
+    <t>NO_HTTP_METHOD_DEFINED</t>
+  </si>
+  <si>
+    <t>Each "RESTOperation" must define at least one HTTP method. If this message occurs then you have to fix your UML Model.</t>
+  </si>
+  <si>
+    <t>INVALID_HTTP_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>The "RESTOperation" uses a HTTP status code that is not compatible with JAX-RS standard.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» uses http status code ''{0}'' which is not compatible with JAX-RS.</t>
+  </si>
+  <si>
+    <t>NO_CONSUMED_MEDIA_TYPE_DEFINED</t>
+  </si>
+  <si>
+    <t>The supported consumed media types can either be defined on the "RESTResource" or on the "RESTOperation" but at least on one of them the information has to be defined.</t>
+  </si>
+  <si>
+    <t>NO_PRODUCED_MEDIA_TYPE_DEFINED</t>
+  </si>
+  <si>
+    <t>The produced media types can either be defined on the "RESTResource" or on the "RESTOperation" but at least on one of them the information has to be defined.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» ''{0}(...)'' must define at least one HTTP-Method. Please correct your UML model.</t>
+  </si>
+  <si>
+    <t>For «RESTOperation» ''{0}(...)'' no consumed media type is defined. The information can be defined either on the «RESTResource» or «RESTOperation».</t>
+  </si>
+  <si>
+    <t>For «RESTOperation» ''{0}(...)'' no produced media type is defined. The information can be defined either on the «RESTResource» or «RESTOperation».</t>
+  </si>
+  <si>
+    <t>«RESTOperation» ''{0}(...)'' has input parameters without name. Please ensure that all input parameters are named.</t>
+  </si>
+  <si>
+    <t>REST_INPUT_PARAM_WITHOUT_NAME</t>
+  </si>
+  <si>
+    <t>All input paramaters of a "RESTOperation" have to have a name. Please fix the issue in your UML model.</t>
+  </si>
+  <si>
+    <t>MULTIPLE_REQUEST_BODIES</t>
+  </si>
+  <si>
+    <t>«RESTOperation» ''{0}(...)'' has multiple request body parameters. Please ensure that there is not more than 1 request body for a REST operation. The following paramaters are treated as body parameters: {1}</t>
+  </si>
+  <si>
+    <t>All input paramaters that are not explicitly marked as "HeaderParam", "PathParam", "BeanParam" etc. are treated as body. However REST only supports one body per request. So please ensure that there is not more than 1 body per request.</t>
+  </si>
+  <si>
+    <t>REQUEST_BODY_NOT_ALLOWED</t>
+  </si>
+  <si>
+    <t>A "RESTOperation" defines a body paramater, however it's HTTP method does not allow to use a body.</t>
+  </si>
+  <si>
+    <t>MORE_THAN_ONE_GLOBAL_ERROR_RESPONSE</t>
+  </si>
+  <si>
+    <t>UML Model contains has more than one global default error response.</t>
+  </si>
+  <si>
+    <t>It's not allowed to have more than 1 global error reponse for an OpenAPI specification in an UML Model.</t>
+  </si>
+  <si>
+    <t>TO_MANY_OPEN_API_RESPONSE_TYPES</t>
+  </si>
+  <si>
+    <t>"OpenAPIResponse" types need to define exactly one response type</t>
+  </si>
+  <si>
+    <t>«OpenAPIResponse» ''{0}'' needs to define exactly one reference to «OpenAPIType» that is used as response type.</t>
+  </si>
+  <si>
+    <t>"OpenAPIDataType" must have 1 property as long as they are not modeled as composite data types.</t>
+  </si>
+  <si>
+    <t>OPEN_API_DATA_TYPE_TOO_MANY_PROPERTIES</t>
+  </si>
+  <si>
+    <t>OPEN_API_DATA_TYPE_ONLY_PRIMITIVES</t>
+  </si>
+  <si>
+    <t>"OpenAPIDataType" must only have primitive types of properties, as long as they are not modeled as composite data types.</t>
+  </si>
+  <si>
+    <t>OPEN_API_DATA_TYPE_NO_MULTIVALUED_PROPERTIES</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» ''{0}'' must have excatly one property as long as they are not marked as composite data types.</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» ''{0}'' has property that is not a primitive.</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» ''{0}'' must not have multivalued properties.</t>
+  </si>
+  <si>
+    <t>"OpenAPIDataType" must not have multivalued properties, as long as they are not modeled as composite data types.</t>
+  </si>
+  <si>
+    <t>OPEN_API_DATA_TYPE_PARENT_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» ''{0}'' must not have a prante class.</t>
+  </si>
+  <si>
+    <t>"OpenAPIDataType" must not have parent classes.</t>
+  </si>
+  <si>
+    <t>PATH_PARAM_MUST_BE_REQUIRED</t>
+  </si>
+  <si>
+    <t>When defining a path param for a "RESTOperation" it is required that path paramaters are required.</t>
+  </si>
+  <si>
+    <t>«PathParam» ''{0}'' needs to be defined as required in the UML Model.</t>
+  </si>
+  <si>
+    <t>PATH_PARAM_MUST_NOT_BE_MULTIVALUED</t>
+  </si>
+  <si>
+    <t>"PathParam" must not be defined as multivalued in the UML Model.</t>
+  </si>
+  <si>
+    <t>«PathParam» ''{0}'' must not be defined as multivalued in the UML Model.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» ''{0}(...)'' has request body parameter even though its http method(s) ''{1}'' do(es) not allow it.</t>
+  </si>
+  <si>
+    <t>DOCUMENTATION_MISSING</t>
+  </si>
+  <si>
+    <t>It is strongly recommended that the elements of the UML model have a meaningful documentation ;-)</t>
+  </si>
+  <si>
+    <t>«{0}» ''{1}'' should have a documentation in the UML model.</t>
+  </si>
+  <si>
+    <t>NO_PARENT_FOR_COMPOSITE_DATA_TYPES</t>
+  </si>
+  <si>
+    <t>When working with so called composite data types then inherhitance is not suppported for them.</t>
+  </si>
+  <si>
+    <t>«{0}» ''{1}'' must not have a parent class as it is marked to be a composite data type.</t>
   </si>
 </sst>
 </file>
@@ -845,51 +1025,51 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C78FBD0B-2020-4712-86AE-D7BCE8E6B516}" name="Tabelle145" displayName="Tabelle145" ref="A1:I101" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C78FBD0B-2020-4712-86AE-D7BCE8E6B516}" name="Tabelle145" displayName="Tabelle145" ref="A1:I101" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7537072B-DA19-4318-B7AA-14135B307274}" name="Message-ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F323142C-244E-41F1-93A6-0AA08BE7B8FF}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{AF060E36-B6B7-4892-8622-D50FCC5AE8CD}" name="Message-Type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{0654D6ED-D6B6-4967-8B32-955A11DEDA63}" name="Trace-Level" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{ED3A71A8-CA63-40A0-BEDA-3FDF4E2F8316}" name="Deprecated" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{22FBD96D-7809-44EA-9E67-2F10C6A009AE}" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E825B3A2-5DED-420D-AB44-AB28640EE14E}" name="Default-Text" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{9FDD04FF-3345-4296-824C-3195B380304A}" name="de" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{5A1A78E9-A7C9-4DAD-9525-03A8700CD71F}" name="de_CH" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7537072B-DA19-4318-B7AA-14135B307274}" name="Message-ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{F323142C-244E-41F1-93A6-0AA08BE7B8FF}" name="Name" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{AF060E36-B6B7-4892-8622-D50FCC5AE8CD}" name="Message-Type" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{0654D6ED-D6B6-4967-8B32-955A11DEDA63}" name="Trace-Level" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{ED3A71A8-CA63-40A0-BEDA-3FDF4E2F8316}" name="Deprecated" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{22FBD96D-7809-44EA-9E67-2F10C6A009AE}" name="Description" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{E825B3A2-5DED-420D-AB44-AB28640EE14E}" name="Default-Text" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9FDD04FF-3345-4296-824C-3195B380304A}" name="de" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{5A1A78E9-A7C9-4DAD-9525-03A8700CD71F}" name="de_CH" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{948296A2-6F04-4C20-9E8E-5BB5FABA5A70}" name="Tabelle14" displayName="Tabelle14" ref="A1:I45" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{948296A2-6F04-4C20-9E8E-5BB5FABA5A70}" name="Tabelle14" displayName="Tabelle14" ref="A1:I45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{967D6801-B5F2-4970-A27A-F85C37854D60}" name="Message-ID" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{88E5ADDA-3853-468E-B030-85021C9A6650}" name="Name" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{740749F7-6FAA-4481-BC95-7F1796A2432D}" name="Message-Type" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{19311204-5730-4A79-9D38-7FC86468DF77}" name="Trace-Level" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{3E8ADF41-0BB1-4927-B4B6-18C125FBAB4D}" name="Deprecated" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{6165C651-89C2-47C8-9C0A-7E31E39C3BDC}" name="Description" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{C07594BE-26A2-446A-9EEB-CCB78235D1A1}" name="Default-Text" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{B4B20E49-AADE-4F41-BEBA-FA3CF75FE9C4}" name="de" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{996AA4AD-7F15-4AE4-AF3A-25B3F210F094}" name="de_CH" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{967D6801-B5F2-4970-A27A-F85C37854D60}" name="Message-ID" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{88E5ADDA-3853-468E-B030-85021C9A6650}" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{740749F7-6FAA-4481-BC95-7F1796A2432D}" name="Message-Type" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{19311204-5730-4A79-9D38-7FC86468DF77}" name="Trace-Level" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{3E8ADF41-0BB1-4927-B4B6-18C125FBAB4D}" name="Deprecated" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{6165C651-89C2-47C8-9C0A-7E31E39C3BDC}" name="Description" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{C07594BE-26A2-446A-9EEB-CCB78235D1A1}" name="Default-Text" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{B4B20E49-AADE-4F41-BEBA-FA3CF75FE9C4}" name="de" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{996AA4AD-7F15-4AE4-AF3A-25B3F210F094}" name="de_CH" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CA772BD-8BBC-4A69-B04B-07ABC6834AB5}" name="Tabelle1" displayName="Tabelle1" ref="A1:I45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CA772BD-8BBC-4A69-B04B-07ABC6834AB5}" name="Tabelle1" displayName="Tabelle1" ref="A1:I45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{99B83EAC-0470-4BBD-BF0F-0B3ED216B509}" name="Message-ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1D0805BB-14A5-46D8-926C-7EF19373398A}" name="Name" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{95D9BE1F-E505-4244-BF73-730083595171}" name="Message-Type" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{3AEE1724-EB57-4317-9B44-58142DC5CE51}" name="Trace-Level" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{BCBCDD70-00BD-4A71-AB02-AEADBAA7CE21}" name="Deprecated" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{8A4D2204-43F3-40F6-BF3B-9C6E5AB6BCD1}" name="Description" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{5D2E8F0C-58F0-4394-8334-DBCC1FF18746}" name="Default-Text" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{ECEC86C7-BC45-4B18-80E4-4C2F755B8A25}" name="de" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{A2C4A677-579B-412F-A217-B5C30A83C750}" name="de_CH" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{99B83EAC-0470-4BBD-BF0F-0B3ED216B509}" name="Message-ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1D0805BB-14A5-46D8-926C-7EF19373398A}" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{95D9BE1F-E505-4244-BF73-730083595171}" name="Message-Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{3AEE1724-EB57-4317-9B44-58142DC5CE51}" name="Trace-Level" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{BCBCDD70-00BD-4A71-AB02-AEADBAA7CE21}" name="Deprecated" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{8A4D2204-43F3-40F6-BF3B-9C6E5AB6BCD1}" name="Description" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5D2E8F0C-58F0-4394-8334-DBCC1FF18746}" name="Default-Text" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{ECEC86C7-BC45-4B18-80E4-4C2F755B8A25}" name="de" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{A2C4A677-579B-412F-A217-B5C30A83C750}" name="de_CH" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1217,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D2429C-A9DF-4A1D-9766-3D100868C9B7}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1314,7 +1494,7 @@
         <v>9000</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1323,10 +1503,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1334,7 +1514,7 @@
         <v>9001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1343,10 +1523,10 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1354,7 +1534,7 @@
         <v>9002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -1363,10 +1543,10 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1374,7 +1554,7 @@
         <v>9003</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -1383,10 +1563,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1394,7 +1574,7 @@
         <v>9004</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -1403,10 +1583,10 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1414,7 +1594,7 @@
         <v>9005</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -1423,10 +1603,10 @@
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1434,7 +1614,7 @@
         <v>9006</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -1443,10 +1623,10 @@
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1454,7 +1634,7 @@
         <v>9007</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
@@ -1463,10 +1643,10 @@
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1474,7 +1654,7 @@
         <v>9008</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
@@ -1483,10 +1663,10 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1494,7 +1674,7 @@
         <v>9009</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -1503,10 +1683,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1514,7 +1694,7 @@
         <v>9010</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -1523,10 +1703,10 @@
         <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1534,7 +1714,7 @@
         <v>9011</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
@@ -1543,10 +1723,10 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1554,7 +1734,7 @@
         <v>9012</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
@@ -1563,10 +1743,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1574,7 +1754,7 @@
         <v>9013</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -1583,10 +1763,10 @@
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2062,16 +2242,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
     <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="1"/>
@@ -2123,7 +2304,7 @@
         <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2143,7 +2324,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2163,7 +2344,7 @@
         <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2183,140 +2364,440 @@
         <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9104</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>9105</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>9106</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9107</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9108</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9109</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9110</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9111</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9112</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9113</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9114</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9115</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9116</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9117</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>9118</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9119</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>9120</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>9121</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9122</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>9123</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9124</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9125</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>9126</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>9127</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>9128</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>9129</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>9130</v>
       </c>
@@ -2411,7 +2892,7 @@
           <x14:formula1>
             <xm:f>'Predefined-Values'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D45 E3:E45</xm:sqref>
+          <xm:sqref>E3:E45 D2:D45</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00450C44-2AB6-4CEB-9EFF-8550DB68F674}">
           <x14:formula1>

</xml_diff>

<commit_message>
Added some more messages
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030BA0AB-42E0-4242-AA44-F835FBE212A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57233710-848E-4991-B73C-9B4F7ADD001A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="157">
   <si>
     <t>Class-Info</t>
   </si>
@@ -728,6 +728,24 @@
   </si>
   <si>
     <t>«OpenAPIDataType» ''{0}'' must not have a parent class.</t>
+  </si>
+  <si>
+    <t>INVALID_SERVICE_RETURN_TYPE</t>
+  </si>
+  <si>
+    <t>When modelling operations of services it is required that they also have a return type. Also case "void" has to be defined in UML Model. In addition multivalued primitive types are not supported as return types.</t>
+  </si>
+  <si>
+    <t>«JEAFService» ''{0}'' has method(s) with unsupported return type. Please ensure that all methods have a real return type and that no arrays of primitive types returned.</t>
+  </si>
+  <si>
+    <t>INPUT_PARAMS_WITHOUT_NAME</t>
+  </si>
+  <si>
+    <t>When modelling parameters of operations it is reuiqred that they also have a name. If there are input parameters without a name then code generation is not possible.</t>
+  </si>
+  <si>
+    <t>«{0}» ''{1}'' has method(s) with input parameters without name. Please ensure that all input parameters in every method are named in the UML Model.</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +2279,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,14 +2843,44 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>9126</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>9127</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JEAF-3109 All messages migrated
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1965EA-C87D-4894-80CD-48EA18DB0BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055ED177-6889-4815-B4D6-EB2C0C6FE1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="229">
   <si>
     <t>Class-Info</t>
   </si>
@@ -827,6 +827,141 @@
   </si>
   <si>
     <t>«ObjectMapping» between properties ''{0}'' and ''{1}'' is invalid. {2}</t>
+  </si>
+  <si>
+    <t>Minimum value for for Java Bean Validation "DecimalMin" is missing.</t>
+  </si>
+  <si>
+    <t>WRONG_TARGET_TYPE_STRING_OR_NUMBER</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». CharcterSequence or number is expected.</t>
+  </si>
+  <si>
+    <t>Maximum value for for Java Bean Validation "DecimalMax" is missing.</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a string-based or numeric target type is expected.</t>
+  </si>
+  <si>
+    <t>DECIMAL_MIN_VALUE_MISSING</t>
+  </si>
+  <si>
+    <t>DECIMAL_MAX_VALUE_MISSING</t>
+  </si>
+  <si>
+    <t>WRONG_TARGET_TYPE_NUMBER</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a numeric target type is expected.</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». Number is expected.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Digit" then the integral and fractional digits have to be defined properly.</t>
+  </si>
+  <si>
+    <t>WRONG_INTEGER_DIGITS</t>
+  </si>
+  <si>
+    <t>WRONG_FRACTIONAL_DIGITS</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Digits" then the integral and fractional digits have to be defined properly.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid value. Minimum size for Java Bean Validation «Size» must be zero or greater (min = {1}).</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid number of integral digits for Java Bean Validation «Digits». Value must be zero or greater (integer = {1}).</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid number of fractional digits for Java Bean Validation «Digits». Value must be zero or greater (fraction = {1}).</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid value. Maximum size for Java Bean Validation «Size» must be greater or equal as minimum size (min = {1}  max = {2}).</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid value. Either maximum or minimum size of Java Bean Validation «Size» must be set.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Size" then ist minimal size has to be set properly.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has invalid value. Maximum size for Java Bean Validation «Size» must be zero or greater (max = {1}).</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Size" then ist maximum size has to be set properly.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Size" then at least minimum or maximum size has to be set.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Size" maximum size has to be greater or equal to minimum size.</t>
+  </si>
+  <si>
+    <t>INVALID_SIZE_MIN</t>
+  </si>
+  <si>
+    <t>INVALID_SIZE_MAX</t>
+  </si>
+  <si>
+    <t>INVALID_MAX_MIN_SIZE</t>
+  </si>
+  <si>
+    <t>EITHER_MIN_OR_MAX_HAS_TO_BE_SET</t>
+  </si>
+  <si>
+    <t>WRONG_TYPE_CHAR_OR_CONTAINER</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a string, collection and map target type is expected.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' has defined Java Bean Validation «Pattern» but no regexp pattern is defined in UML model.</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a string target type is expected.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation "Pattern" then a regexp pattern has to be set.</t>
+  </si>
+  <si>
+    <t>REGEXP_PATTERN_MISSING</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a boolean target type is expected.</t>
+  </si>
+  <si>
+    <t>WRONG_TYPE_BOOLEAN</t>
+  </si>
+  <si>
+    <t>For a specific Java Bean Validation a date target type is expected.</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». Date is expected.</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». Boolean is expected.</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». CharcterSequence is expected.</t>
+  </si>
+  <si>
+    <t>Wrong target type ''{0}'' for Java Bean Validation «{1}». CharcterSequence, Collection or Map is expected.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' does not define a minimum value even though it uses Java Bean Validation «DecimalMin».</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' does not define a maximum value even though it uses Java Bean Validation «DecimalMax»."</t>
+  </si>
+  <si>
+    <t>WRONG_TYPE_DATE</t>
+  </si>
+  <si>
+    <t>WRONG_TYPE_CHAR</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1294,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{948296A2-6F04-4C20-9E8E-5BB5FABA5A70}" name="Tabelle14" displayName="Tabelle14" ref="A1:I45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{948296A2-6F04-4C20-9E8E-5BB5FABA5A70}" name="Tabelle14" displayName="Tabelle14" ref="A1:I101" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{967D6801-B5F2-4970-A27A-F85C37854D60}" name="Message-ID" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{88E5ADDA-3853-468E-B030-85021C9A6650}" name="Name" dataDxfId="18"/>
@@ -2357,10 +2492,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,44 +3279,549 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>9137</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>9138</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>9139</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>9140</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>9141</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>9142</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>9143</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>9144</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>9145</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>9146</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>9147</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>9148</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>9149</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>9150</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>9151</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>9152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>9153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>9154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>9155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>9156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>9157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>9158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>9159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>9160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>9161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>9162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>9163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>9164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>9165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>9166</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>9167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>9168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>9169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>9170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>9171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>9172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>9173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>9174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>9175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>9176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>9177</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>9178</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>9179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>9180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>9181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>9182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>9183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>9185</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>9187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>9188</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>9189</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>9190</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>9191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>9192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>9193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>9194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>9195</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>9196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>9197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>9198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>9199</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A45" xr:uid="{AACEF8C0-EC92-4686-A8C3-E4036D94D483}">
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A101" xr:uid="{AACEF8C0-EC92-4686-A8C3-E4036D94D483}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -3193,7 +3833,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EA474BAA-D9F0-48C4-BFC6-D7532DADFCD0}">
           <x14:formula1>
             <xm:f>'Predefined-Values'!$C$4:$C$5</xm:f>
@@ -3204,13 +3844,13 @@
           <x14:formula1>
             <xm:f>'Predefined-Values'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E45 D2:D45</xm:sqref>
+          <xm:sqref>E3:E45 D2:D101</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00450C44-2AB6-4CEB-9EFF-8550DB68F674}">
           <x14:formula1>
             <xm:f>'Predefined-Values'!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C45</xm:sqref>
+          <xm:sqref>C2:C101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixed spelling bugs in descriptions of errors.
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9634B59A-B376-4831-A566-09AA1A029D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9675D4-882B-420D-9D0D-58AD66A42710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -625,9 +625,6 @@
     <t>NO_PARENT_FOR_COMPOSITE_DATA_TYPES</t>
   </si>
   <si>
-    <t>When working with so called composite data types then inherhitance is not suppported for them.</t>
-  </si>
-  <si>
     <t>«{0}» ''{1}'' must not have a parent class as it is marked to be a composite data type.</t>
   </si>
   <si>
@@ -841,15 +838,6 @@
     <t>The produced media types can either be defined on the «RESTResource» or on the «RESTOperation» but at least on one of them the information has to be defined.</t>
   </si>
   <si>
-    <t>All input paramaters of a «RESTOperation» must hava a name. Please fix the issue in your UML model.</t>
-  </si>
-  <si>
-    <t>All input paramaters that are not explicitly marked as «HeaderParam», «PathParam», «BeanParam» etc. are treated as body. However REST only supports one body per request. So please ensure that there is not more than 1 body per request.</t>
-  </si>
-  <si>
-    <t>A «RESTOperation» defines a body paramater, however it's HTTP method does not allow to use a body.</t>
-  </si>
-  <si>
     <t>«OpenAPIResponse» types need to define exactly one response type</t>
   </si>
   <si>
@@ -859,18 +847,9 @@
     <t>«OpenAPIDataType» must only have primitive types of properties, as long as they are not modeled as composite data types.</t>
   </si>
   <si>
-    <t>«OpenAPIDataType» must not have multivalued properties, as long as they are not modeled as composite data types.</t>
-  </si>
-  <si>
     <t>«OpenAPIDataType» must not have parent classes.</t>
   </si>
   <si>
-    <t>When defining a path param for a «RESTOperation» it is required that path paramaters are required.</t>
-  </si>
-  <si>
-    <t>«PathParam» must not be defined as multivalued in the UML model.</t>
-  </si>
-  <si>
     <t>«ObjectMapping» is invalid according to the error message</t>
   </si>
   <si>
@@ -886,12 +865,6 @@
     <t>When working with Java Bean Validation «Digits» then the integral and fractional digits have to be defined properly.</t>
   </si>
   <si>
-    <t>When working with Java Bean Validation «Size» then ist minimal size has to be set properly.</t>
-  </si>
-  <si>
-    <t>When working with Java Bean Validation «Size» then ist maximum size has to be set properly.</t>
-  </si>
-  <si>
     <t>When working with Java Bean Validation «Size» maximum size has to be greater or equal to minimum size.</t>
   </si>
   <si>
@@ -907,9 +880,6 @@
     <t>Each «RESTOperation» must define at least one HTTP method. If this message occurs then you have to fix your UML model.</t>
   </si>
   <si>
-    <t>It's not allowed to have more than 1 global error reponse for an OpenAPI specification in an UML model.</t>
-  </si>
-  <si>
     <t>UML model contains has more than one global default error response.</t>
   </si>
   <si>
@@ -943,15 +913,6 @@
     <t>When modeling attributes in UML it is important that they also have a type. If a type is not defined then code generation is not possible.</t>
   </si>
   <si>
-    <t>When modeling attributes and associations then it is reuiqred that they also have a type. If it is not defined then code generation is not possible.</t>
-  </si>
-  <si>
-    <t>When modeling operations of services it is required that they also have a return type. Also case "void" has to be defined in UML model. In addition multivalued primitive types are not supported as return types.</t>
-  </si>
-  <si>
-    <t>When modeling parameters of operations it is reuiqred that they also have a name. If there are input parameters without a name then code generation is not possible.</t>
-  </si>
-  <si>
     <t>When modeling methods also a return type is required not only for methods that really return something but also in case of "void". If a method does not define a return type then code generation is not possible.</t>
   </si>
   <si>
@@ -962,6 +923,45 @@
   </si>
   <si>
     <t>When modeling «JEAFComponents» you have to ensure that each component has defined a layer.</t>
+  </si>
+  <si>
+    <t>All input parameters that are not explicitly marked as «HeaderParam», «PathParam», «BeanParam» etc. are treated as body. However REST only supports one body per request. So please ensure that there is not more than 1 body per request.</t>
+  </si>
+  <si>
+    <t>A «RESTOperation» defines a body parameter, however it's HTTP method does not allow to use a body.</t>
+  </si>
+  <si>
+    <t>It's not allowed to have more than 1 global error response for an OpenAPI specification in an UML model.</t>
+  </si>
+  <si>
+    <t>All input parameters of a «RESTOperation» must have a name. Please fix the issue in your UML model.</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» must not have multi valued properties, as long as they are not modeled as composite data types.</t>
+  </si>
+  <si>
+    <t>When defining a «PathParam» for a «RESTOperation» it is required that path parameters are required.</t>
+  </si>
+  <si>
+    <t>When working with so called composite data types then inheritance is not supported for them.</t>
+  </si>
+  <si>
+    <t>«PathParam» must not be defined as multi valued in the UML model.</t>
+  </si>
+  <si>
+    <t>When modeling attributes and associations then it is required that they also have a type. If it is not defined then code generation is not possible.</t>
+  </si>
+  <si>
+    <t>When modeling operations of services it is required that they also have a return type. Also case "void" has to be defined in UML model. In addition multi valued primitive types are not supported as return types.</t>
+  </si>
+  <si>
+    <t>When modeling parameters of operations it is required that they also have a name. If there are input parameters without a name then code generation is not possible.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation «Size» then its minimal size has to be set properly.</t>
+  </si>
+  <si>
+    <t>When working with Java Bean Validation «Size» then its maximum size has to be set properly.</t>
   </si>
 </sst>
 </file>
@@ -2494,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2553,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>80</v>
@@ -2576,7 +2576,7 @@
         <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>38</v>
@@ -2613,10 +2613,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>85</v>
@@ -2653,7 +2653,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>83</v>
@@ -2673,7 +2673,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>84</v>
@@ -2693,7 +2693,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>91</v>
@@ -2713,7 +2713,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>88</v>
@@ -2733,7 +2733,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>92</v>
@@ -2753,7 +2753,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>93</v>
@@ -2773,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>94</v>
@@ -2793,7 +2793,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>97</v>
@@ -2813,7 +2813,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>111</v>
@@ -2833,10 +2833,10 @@
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>101</v>
@@ -2873,7 +2873,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>105</v>
@@ -2893,7 +2893,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>106</v>
@@ -2913,7 +2913,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>107</v>
@@ -2933,10 +2933,10 @@
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2953,10 +2953,10 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2973,10 +2973,10 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>9124</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -3033,10 +3033,10 @@
         <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>9125</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
@@ -3053,10 +3053,10 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3064,19 +3064,19 @@
         <v>9126</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
         <v>9127</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -3093,10 +3093,10 @@
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3104,19 +3104,19 @@
         <v>9128</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>9129</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -3133,10 +3133,10 @@
         <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3144,19 +3144,19 @@
         <v>9130</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>9131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
@@ -3173,10 +3173,10 @@
         <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3184,19 +3184,19 @@
         <v>9132</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3204,19 +3204,19 @@
         <v>9133</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3224,19 +3224,19 @@
         <v>9134</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3244,19 +3244,19 @@
         <v>9135</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3264,19 +3264,19 @@
         <v>9136</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3284,7 +3284,7 @@
         <v>9137</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -3293,10 +3293,10 @@
         <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3304,19 +3304,19 @@
         <v>9138</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
         <v>9139</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
@@ -3333,10 +3333,10 @@
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3344,19 +3344,19 @@
         <v>9140</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3364,7 +3364,7 @@
         <v>9141</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>12</v>
@@ -3373,10 +3373,10 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>9142</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>12</v>
@@ -3393,10 +3393,10 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3404,7 +3404,7 @@
         <v>9143</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>12</v>
@@ -3413,10 +3413,10 @@
         <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
         <v>9144</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -3433,10 +3433,10 @@
         <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3444,7 +3444,7 @@
         <v>9145</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -3453,10 +3453,10 @@
         <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
         <v>9146</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>12</v>
@@ -3473,10 +3473,10 @@
         <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3484,19 +3484,19 @@
         <v>9147</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="G49" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>9148</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>12</v>
@@ -3513,10 +3513,10 @@
         <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
         <v>9149</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -3533,10 +3533,10 @@
         <v>12</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
         <v>9150</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>12</v>
@@ -3553,10 +3553,10 @@
         <v>12</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3564,7 +3564,7 @@
         <v>9151</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>12</v>
@@ -3573,10 +3573,10 @@
         <v>12</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Extended message for JEAF-3125
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9FBAF0-2731-419E-B201-EAE302C33119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB925E0B-EBBA-406E-BA6D-C7029AFC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="235">
   <si>
     <t>Class-Info</t>
   </si>
@@ -971,6 +971,17 @@
   </si>
   <si>
     <t>Special stereotype «Ignore» can be used to explicitly exclude model elements from code generation. However this mechanism is intended to be a workaround / short term solution and not a permanent one ;-). Proper solution to this is to clean up your UML model. That's why a warning is shown during code generation.</t>
+  </si>
+  <si>
+    <t>IGNOREABLE_OPEN_API_HEADER_FOUND</t>
+  </si>
+  <si>
+    <t>OpenAPI standard defines that for whatever reason some header fileds should not be mentioned in the OpenAPI specification e.g. ''Authorization'' header. However from an overall perspective it still might make sense to explicitly model them e.g. if these fields are still required in Java code.
+Putting it all together in very most cases this warning can be ignored and is only generated to empahsis that these headers did not get "forgotten" in generation of OpenAPI specification but are not added by intention.
+For further details please also refer to https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject</t>
+  </si>
+  <si>
+    <t>Operation / Bean Param ''{0}'' defines a http header field ''{1}'' using parameter / property ''{2}''. According to ''https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject'' header fields with this name should not be added to an OpenAPI specification. This is not an issue. However the header field will not be present in the generated OpenAPI specification.</t>
   </si>
 </sst>
 </file>
@@ -2503,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,9 +3619,24 @@
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>9153</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JEAF-3125 Fixed error message
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB925E0B-EBBA-406E-BA6D-C7029AFC2C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70260B12-F5C8-4ACB-A705-209A3087292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -976,12 +976,12 @@
     <t>IGNOREABLE_OPEN_API_HEADER_FOUND</t>
   </si>
   <si>
-    <t>OpenAPI standard defines that for whatever reason some header fileds should not be mentioned in the OpenAPI specification e.g. ''Authorization'' header. However from an overall perspective it still might make sense to explicitly model them e.g. if these fields are still required in Java code.
-Putting it all together in very most cases this warning can be ignored and is only generated to empahsis that these headers did not get "forgotten" in generation of OpenAPI specification but are not added by intention.
+    <t>Operation / Bean Param ''{0}'' defines a http header field ''{1}'' using parameter / property ''{2}''. According to ''https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject'' header fields with this name should not be added to an OpenAPI specification. This is not an issue. However the header field will not be present in the generated OpenAPI specification.</t>
+  </si>
+  <si>
+    <t>OpenAPI standard defines that for whatever reason some header fields should not be mentioned in the OpenAPI specification e.g. ''Authorization'' header. However from an overall perspective it still might make sense to explicitly model them e.g. if these fields are still required in Java code.
+Putting it all together in very most cases this warning can be ignored and is only generated to emphasis that these headers did not get "forgotten" in generation of OpenAPI specification but are not added by intention.
 For further details please also refer to https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject</t>
-  </si>
-  <si>
-    <t>Operation / Bean Param ''{0}'' defines a http header field ''{1}'' using parameter / property ''{2}''. According to ''https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject'' header fields with this name should not be added to an OpenAPI specification. This is not an issue. However the header field will not be present in the generated OpenAPI specification.</t>
   </si>
 </sst>
 </file>
@@ -2515,7 +2515,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3633,10 +3633,10 @@
         <v>15</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JEAF-3155: Added error message
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70260B12-F5C8-4ACB-A705-209A3087292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F02F526-8B64-4A60-8631-58E31E94BFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="237">
   <si>
     <t>Class-Info</t>
   </si>
@@ -862,9 +862,6 @@
     <t>When working with Java Bean Validation «Digit» then the integral and fractional digits have to be defined properly.</t>
   </si>
   <si>
-    <t>When working with Java Bean Validation «Digits» then the integral and fractional digits have to be defined properly.</t>
-  </si>
-  <si>
     <t>When working with Java Bean Validation «Size» maximum size has to be greater or equal to minimum size.</t>
   </si>
   <si>
@@ -968,9 +965,6 @@
   </si>
   <si>
     <t>Model element ''{0}'' is marked to be ignored. Please ensure that this is still fine. Stereotype «Ignore» is intended to be a short term solution to exclude model elements.</t>
-  </si>
-  <si>
-    <t>Special stereotype «Ignore» can be used to explicitly exclude model elements from code generation. However this mechanism is intended to be a workaround / short term solution and not a permanent one ;-). Proper solution to this is to clean up your UML model. That's why a warning is shown during code generation.</t>
   </si>
   <si>
     <t>IGNOREABLE_OPEN_API_HEADER_FOUND</t>
@@ -982,6 +976,22 @@
     <t>OpenAPI standard defines that for whatever reason some header fields should not be mentioned in the OpenAPI specification e.g. ''Authorization'' header. However from an overall perspective it still might make sense to explicitly model them e.g. if these fields are still required in Java code.
 Putting it all together in very most cases this warning can be ignored and is only generated to emphasis that these headers did not get "forgotten" in generation of OpenAPI specification but are not added by intention.
 For further details please also refer to https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject</t>
+  </si>
+  <si>
+    <t>DEPRECATION_MARKING_NOT_ALLOWED</t>
+  </si>
+  <si>
+    <t>Special stereotype «Ignore» can be used to explicitly exclude model elements from code generation. However this mechanism is intended to be a workaround / short term solution and not a permanent one ;-). 
+Proper solution to this is to clean up your UML model. That's why a warning is shown during code generation.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' is marked as deprecated. However OpenAPI does not support to mark references to complex types as deprecated.</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports to mark various elements in the UML model as deprecated. This information is also added to the generated code and OpenAPI specification.
+However, there are cases where OpenAPI does not allow to mark an element as deprecated. Namely this is the case for single valued references to other complex types like a 0..1 association to another object. In this case the generated Java code will still contain the deprecation but the OpenAPI specification will not have "deprecation: true". Instead only as comment inside the file is created. 
+Example:
+- # Property "xyz" is marked as deprecated. However OpenAPI does not support to mark references to complex types as deprecated.</t>
   </si>
 </sst>
 </file>
@@ -2514,7 +2524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
@@ -2573,7 +2583,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>80</v>
@@ -2613,7 +2623,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>38</v>
@@ -2713,7 +2723,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>91</v>
@@ -2793,7 +2803,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>94</v>
@@ -2813,7 +2823,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>97</v>
@@ -2833,7 +2843,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>111</v>
@@ -2853,10 +2863,10 @@
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2933,7 +2943,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>107</v>
@@ -2973,10 +2983,10 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2993,10 +3003,10 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3033,7 +3043,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>116</v>
@@ -3053,10 +3063,10 @@
         <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3073,10 +3083,10 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3093,7 +3103,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>121</v>
@@ -3113,10 +3123,10 @@
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3133,7 +3143,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>124</v>
@@ -3153,7 +3163,7 @@
         <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>128</v>
@@ -3193,7 +3203,7 @@
         <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>133</v>
@@ -3213,7 +3223,7 @@
         <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>132</v>
@@ -3233,7 +3243,7 @@
         <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>137</v>
@@ -3253,7 +3263,7 @@
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>139</v>
@@ -3273,7 +3283,7 @@
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>141</v>
@@ -3413,7 +3423,7 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>156</v>
@@ -3433,7 +3443,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>154</v>
@@ -3453,7 +3463,7 @@
         <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>159</v>
@@ -3473,7 +3483,7 @@
         <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>157</v>
@@ -3493,7 +3503,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>158</v>
@@ -3533,7 +3543,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>166</v>
@@ -3599,12 +3609,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>9152</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>12</v>
@@ -3613,10 +3623,10 @@
         <v>15</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
@@ -3624,7 +3634,7 @@
         <v>9153</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>12</v>
@@ -3633,15 +3643,30 @@
         <v>15</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>9154</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added messages for JEAF-3162
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F02F526-8B64-4A60-8631-58E31E94BFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7FA82-397C-4EB3-800A-1406993C78EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="243">
   <si>
     <t>Class-Info</t>
   </si>
@@ -968,9 +968,6 @@
   </si>
   <si>
     <t>IGNOREABLE_OPEN_API_HEADER_FOUND</t>
-  </si>
-  <si>
-    <t>Operation / Bean Param ''{0}'' defines a http header field ''{1}'' using parameter / property ''{2}''. According to ''https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject'' header fields with this name should not be added to an OpenAPI specification. This is not an issue. However the header field will not be present in the generated OpenAPI specification.</t>
   </si>
   <si>
     <t>OpenAPI standard defines that for whatever reason some header fields should not be mentioned in the OpenAPI specification e.g. ''Authorization'' header. However from an overall perspective it still might make sense to explicitly model them e.g. if these fields are still required in Java code.
@@ -992,6 +989,27 @@
 However, there are cases where OpenAPI does not allow to mark an element as deprecated. Namely this is the case for single valued references to other complex types like a 0..1 association to another object. In this case the generated Java code will still contain the deprecation but the OpenAPI specification will not have "deprecation: true". Instead only as comment inside the file is created. 
 Example:
 - # Property "xyz" is marked as deprecated. However OpenAPI does not support to mark references to complex types as deprecated.</t>
+  </si>
+  <si>
+    <t>COLLECTION_HEADER_PARAM_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>JAX-RS specification only allows to use java.util.List, java.util.Set or java.util.SortedSet for header params but not java.util.Collection. Please fix your UML model so that either List, Set or SortedSet is used for multi valued header fields.</t>
+  </si>
+  <si>
+    <t>COLLECTION_QUERY_PARAM_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>JAX-RS specification only allows to use java.util.List, java.util.Set or java.util.SortedSet for query params but not java.util.Collection. Please fix your UML model so that either List, Set or SortedSet is used for multi valued query params.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» / «BeanParam» ''{0}'' defines a http header field ''{1}'' using parameter / property ''{2}''. According to ''https://github.com/OAI/OpenAPI-Specification/blob/main/versions/3.0.3.md#parameterObject'' header fields with this name should not be added to an OpenAPI specification. This is not an issue. However the header field will not be present in the generated OpenAPI specification.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» / «BeanParam» ''{0}'' defines a java.util.Collection for http header field ''{1}'' using parameter / property ''{2}''. However, JAX-RS sepcification only allows java.util.List, java.util.Set or java.util.SortedSet for headers but not java.util.Collection. Please fix your UML model so that either List, Set or SortedSet is used for multi valued header fields.</t>
+  </si>
+  <si>
+    <t>«RESTOperation» / «BeanParam» ''{0}'' defines a java.util.Collection for query param ''{1}'' using parameter / property ''{2}''. However, JAX-RS sepcification only allows java.util.List, java.util.Set or java.util.SortedSet for query params but not java.util.Collection. Please fix your UML model so that either List, Set or SortedSet is used for multi valued query params.</t>
   </si>
 </sst>
 </file>
@@ -2524,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3623,7 +3641,7 @@
         <v>15</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>229</v>
@@ -3643,10 +3661,10 @@
         <v>15</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -3654,7 +3672,7 @@
         <v>9154</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
@@ -3663,20 +3681,50 @@
         <v>15</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>9155</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>9156</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added messages for JEAF-3113
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA7FA82-397C-4EB3-800A-1406993C78EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F56AF4-5036-4351-8DAB-A80AD557CAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="249">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1010,6 +1010,24 @@
   </si>
   <si>
     <t>«RESTOperation» / «BeanParam» ''{0}'' defines a java.util.Collection for query param ''{1}'' using parameter / property ''{2}''. However, JAX-RS sepcification only allows java.util.List, java.util.Set or java.util.SortedSet for query params but not java.util.Collection. Please fix your UML model so that either List, Set or SortedSet is used for multi valued query params.</t>
+  </si>
+  <si>
+    <t>CUSTOM_GENERIC_TYPE_NOT_CONFIGURED</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports so called soft links. They can be used to modularize your model without loosing information about real types. One possibility when using soft links is to use so called custom generic soft links. In this case you can define your own type that should be used to represent the soft link association. This type, however has to be configured in JEAF Generator Maven Plugin.</t>
+  </si>
+  <si>
+    <t>COMPOSITE_DATA_TYPE_PUBLIC_FIELD_MUST_BE_STRING</t>
+  </si>
+  <si>
+    <t>«CompositeDataTypePublicField» property ''{0}'' is not of type String even though this is required.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' in your UML model makes use of soft links with custom generic types. Please make us of Maven Plugin configuration parameter ''customGenericSoftLinkType''</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports to also make the public representation of a composite data type visible internally. To do so, a property has to be marked with stereotype «CompositeDataTypePublicField». In addition it is required that the property is of type String.</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2542,14 +2560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
@@ -3727,14 +3745,44 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>9157</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>9158</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added message for JEAF-3165
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F56AF4-5036-4351-8DAB-A80AD557CAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42462F56-E34A-4AA5-801D-540C4DE2B91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="252">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1028,6 +1028,15 @@
   </si>
   <si>
     <t>JEAF Generator supports to also make the public representation of a composite data type visible internally. To do so, a property has to be marked with stereotype «CompositeDataTypePublicField». In addition it is required that the property is of type String.</t>
+  </si>
+  <si>
+    <t>OPEN_API_DATA_TYPE_NOT_IMMUTABLE</t>
+  </si>
+  <si>
+    <t>«OpenAPIDataType» ''{0}'' is not immutable. At least one property is not marked as readonly in UML model.</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports so called OpenAPI Data Types. They can be used a strong type representation for basic types. For OpenAPI Data Types it is strongly recommended that they are immutable.</t>
   </si>
 </sst>
 </file>
@@ -2560,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,9 +3794,24 @@
         <v>247</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>9159</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed spelling bug in comment
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCF24B2-BC14-4C4F-BBD5-F2DD5F3D21C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52606B-18DE-479A-8E20-C213797E1AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="255">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1042,10 +1042,10 @@
     <t>EITHER_POJO_OR_SERVICE_OBJECT</t>
   </si>
   <si>
-    <t>And model element can either be marked with stereotype «POJO» or «ServiceObject» but not both of them a teh same time.</t>
-  </si>
-  <si>
     <t>Model element ''{0}'' has applied stereotypes «POJO» and «ServiceObject». However both stereotypes can not be assigned to the same model element at the same time. Please fix your UML model.</t>
+  </si>
+  <si>
+    <t>And model element can either be marked with stereotype «POJO» or «ServiceObject» but not both of them a the same time.</t>
   </si>
 </sst>
 </file>
@@ -2579,7 +2579,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3837,10 +3837,10 @@
         <v>12</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added error message for deprecation report
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52606B-18DE-479A-8E20-C213797E1AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F398F1F-F901-42D2-97D5-DA7CF587E656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="258">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1046,6 +1046,15 @@
   </si>
   <si>
     <t>And model element can either be marked with stereotype «POJO» or «ServiceObject» but not both of them a the same time.</t>
+  </si>
+  <si>
+    <t>INCOMPLETE_DEPRECATION</t>
+  </si>
+  <si>
+    <t>Model element ''{0}'' is marked as deprecated. However at least one of the following information is not provided: "description, "since" or "removedWith"</t>
+  </si>
+  <si>
+    <t>If a model element is marked as deprecated also a description, a "since" flag and the planned removal date of the deprecation should be provided so that consumers of the classes, services etc. can prepare.</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3843,9 +3852,24 @@
         <v>253</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>9161</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JEAF-3177 Added error message
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F398F1F-F901-42D2-97D5-DA7CF587E656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11743BF-0A2F-4136-B9FD-7139C03008D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="261">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1055,6 +1055,15 @@
   </si>
   <si>
     <t>If a model element is marked as deprecated also a description, a "since" flag and the planned removal date of the deprecation should be provided so that consumers of the classes, services etc. can prepare.</t>
+  </si>
+  <si>
+    <t>NO_PUBLIC_FIELD_NAME_FOR_COMPOSITE_DATA_TYPE</t>
+  </si>
+  <si>
+    <t>If a model element is marked as composite data type then a name for the public field representation is required to be set in the model.</t>
+  </si>
+  <si>
+    <t>Composite data type ''{0}'' does not have a public field name configured. Please fix UML model.</t>
   </si>
 </sst>
 </file>
@@ -2587,8 +2596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,9 +3881,24 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>9162</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -4069,7 +4093,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Added new message for JEAF-3142
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11743BF-0A2F-4136-B9FD-7139C03008D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC2F3D-D0B8-4671-BF83-FE6F49ED2A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="264">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1064,6 +1064,15 @@
   </si>
   <si>
     <t>Composite data type ''{0}'' does not have a public field name configured. Please fix UML model.</t>
+  </si>
+  <si>
+    <t>NO_EQUALS_FOR_BIDIRECTIONAL_ASSOCIATIONS</t>
+  </si>
+  <si>
+    <t>Unable to generate equals() and hashCode() for class ''{0}''. The class has at least one bidirectional association.</t>
+  </si>
+  <si>
+    <t>In case that a class has one or more bidirectional associations ist not possible to generate equals() and hashCode() as it requires some business knowledege to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
   </si>
 </sst>
 </file>
@@ -2596,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,82 +3910,97 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>9163</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>9164</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>9165</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>9166</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>9167</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>9168</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>9169</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>9170</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>9171</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>9172</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>9173</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>9174</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>9175</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>9176</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>9177</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>9178</v>
       </c>

</xml_diff>

<commit_message>
Added message for JEAF-3197
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEC2F3D-D0B8-4671-BF83-FE6F49ED2A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EBD67C-4100-44BF-89D2-A816305F33EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="267">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1073,6 +1073,15 @@
   </si>
   <si>
     <t>In case that a class has one or more bidirectional associations ist not possible to generate equals() and hashCode() as it requires some business knowledege to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
+  </si>
+  <si>
+    <t>SOFTLINK_FOR_BIDIRECTIONAL_ASSOCIATION_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports so called soft links. They can be used to modularize and decouple your application. Due to that it does not make sense to use them in combination with bidirectional associations.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' of class ''{1}'' is modeled to be a «SoftLink». However, it belongs to a bidirectional association. Soft links can not be used for bidirectional association as this contradicts to their underlying concept of decoupling.</t>
   </si>
 </sst>
 </file>
@@ -2605,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3930,9 +3939,24 @@
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>9164</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed spelling bugs in new messages
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EBD67C-4100-44BF-89D2-A816305F33EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB92108-6DDD-452D-87CD-1DE5DEB77697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="267">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1072,9 +1072,6 @@
     <t>Unable to generate equals() and hashCode() for class ''{0}''. The class has at least one bidirectional association.</t>
   </si>
   <si>
-    <t>In case that a class has one or more bidirectional associations ist not possible to generate equals() and hashCode() as it requires some business knowledege to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
-  </si>
-  <si>
     <t>SOFTLINK_FOR_BIDIRECTIONAL_ASSOCIATION_NOT_SUPPORTED</t>
   </si>
   <si>
@@ -1082,6 +1079,9 @@
   </si>
   <si>
     <t>Property ''{0}'' of class ''{1}'' is modeled to be a «SoftLink». However, it belongs to a bidirectional association. Soft links can not be used for bidirectional association as this contradicts to their underlying concept of decoupling.</t>
+  </si>
+  <si>
+    <t>In case that a class has one or more bidirectional associations it is not possible to generate equals() and hashCode() as it requires some business knowledge to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
   </si>
 </sst>
 </file>
@@ -2615,7 +2615,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3919,7 +3919,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>9163</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>15</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>262</v>
@@ -3944,19 +3944,19 @@
         <v>9164</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new error messages for JEAF-3102
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB92108-6DDD-452D-87CD-1DE5DEB77697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F417E46-C9FF-43D0-B6AA-5AB2BDD7D1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25590" yWindow="0" windowWidth="25605" windowHeight="21000" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="273">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1082,6 +1082,24 @@
   </si>
   <si>
     <t>In case that a class has one or more bidirectional associations it is not possible to generate equals() and hashCode() as it requires some business knowledge to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
+  </si>
+  <si>
+    <t>A REST operation path defines one or more path params but not all of them are also present as parameters in the defined REST operation</t>
+  </si>
+  <si>
+    <t>Path param(s) ''{0}'' are defined in REST operation with path ''{1}'' but are not defined as parameters / bean parameters in the REST operation ''{2}''.</t>
+  </si>
+  <si>
+    <t>A REST operation defines path parameters that are not defined on the operations paths as parameters</t>
+  </si>
+  <si>
+    <t>PATH_PARAMS_MISSING</t>
+  </si>
+  <si>
+    <t>DEAD_PATH_PARAMS</t>
+  </si>
+  <si>
+    <t>REST operation ''{0}'' with REST path ''{1}'' has at least one path parameter that is not defined in its REST path. Dead parameters: {2}</t>
   </si>
 </sst>
 </file>
@@ -2614,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,14 +3977,44 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>9165</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>9166</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated message 9163 due to feature #80
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F417E46-C9FF-43D0-B6AA-5AB2BDD7D1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB83FD-0704-4A18-8ADD-E0C74629AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="25500" yWindow="0" windowWidth="25785" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -1069,9 +1069,6 @@
     <t>NO_EQUALS_FOR_BIDIRECTIONAL_ASSOCIATIONS</t>
   </si>
   <si>
-    <t>Unable to generate equals() and hashCode() for class ''{0}''. The class has at least one bidirectional association.</t>
-  </si>
-  <si>
     <t>SOFTLINK_FOR_BIDIRECTIONAL_ASSOCIATION_NOT_SUPPORTED</t>
   </si>
   <si>
@@ -1081,9 +1078,6 @@
     <t>Property ''{0}'' of class ''{1}'' is modeled to be a «SoftLink». However, it belongs to a bidirectional association. Soft links can not be used for bidirectional association as this contradicts to their underlying concept of decoupling.</t>
   </si>
   <si>
-    <t>In case that a class has one or more bidirectional associations it is not possible to generate equals() and hashCode() as it requires some business knowledge to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
-  </si>
-  <si>
     <t>A REST operation path defines one or more path params but not all of them are also present as parameters in the defined REST operation</t>
   </si>
   <si>
@@ -1100,6 +1094,12 @@
   </si>
   <si>
     <t>REST operation ''{0}'' with REST path ''{1}'' has at least one path parameter that is not defined in its REST path. Dead parameters: {2}</t>
+  </si>
+  <si>
+    <t>Unable to generate equals() and hashCode() for class ''{0}''. The class has at least one non-transient bidirectional association.</t>
+  </si>
+  <si>
+    <t>In case that a class has one or more non-transient bidirectional associations it is not possible to generate equals() and hashCode() as it requires some business knowledge to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
   </si>
 </sst>
 </file>
@@ -1466,9 +1466,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1506,7 +1506,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1612,7 +1612,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1754,7 +1754,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2632,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3937,7 +3937,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>9163</v>
       </c>
@@ -3951,10 +3951,10 @@
         <v>15</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3962,19 +3962,19 @@
         <v>9164</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
         <v>9165</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>12</v>
@@ -3991,10 +3991,10 @@
         <v>12</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4002,7 +4002,7 @@
         <v>9166</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>12</v>
@@ -4011,10 +4011,10 @@
         <v>15</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added error message for #78
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB83FD-0704-4A18-8ADD-E0C74629AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810158C0-06AF-495F-8679-CDA8714BBA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25500" yWindow="0" windowWidth="25785" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="1560" yWindow="615" windowWidth="25800" windowHeight="20985" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Message-Data-Template" sheetId="2" r:id="rId4"/>
     <sheet name="Predefined-Values" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="279">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1100,6 +1100,24 @@
   </si>
   <si>
     <t>In case that a class has one or more non-transient bidirectional associations it is not possible to generate equals() and hashCode() as it requires some business knowledge to do so. If equals() and hashCode() are required for such a class then it has to be implemented manually.</t>
+  </si>
+  <si>
+    <t>INVALID_TEMPLATE_BINDING_NO_SUBST</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports usage of so called Template Bindings in UML which are an equivalent to generics in Java. If a class makes usage of such a template binding then also a parameter subsitution has to be defined in the UML model.</t>
+  </si>
+  <si>
+    <t>No template binding parameter subsitution defined for class ''{0}''.</t>
+  </si>
+  <si>
+    <t>TOO_MANY_TEMPLATE_BINDINGS</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports usage of so called Template Bindings in UML which are an equivalent to generics in Java. Howver in UML it is possible to define more than one template binding per class. This is currently not supported by JEAF Generator.</t>
+  </si>
+  <si>
+    <t>Class ''{0}'' has more than one template bindung in UML model.</t>
   </si>
 </sst>
 </file>
@@ -2633,7 +2651,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,14 +4035,44 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>9167</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>9168</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added error message for #17
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF709E1-28DD-448F-A797-C53C8D7107B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538B4C69-975B-436A-91E3-3117FB366C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="285">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1133,6 +1133,15 @@
   </si>
   <si>
     <t>JEAF Generator supports usage of so called Template Bindings in UML which are an equivalent to generics in Java. If a class makes usage of such a template binding then also a parameter substitution has to be defined in the UML model.</t>
+  </si>
+  <si>
+    <t>INVALID_IDENTIFIER_NAME</t>
+  </si>
+  <si>
+    <t>Names of classes, enumerations, properties, parameters and operations must match to regular expression according to Java Language Specification.</t>
+  </si>
+  <si>
+    <t>Name ''{0}'' of {1} of ''{2}'' does not match to naming requirements of Java Language specification.</t>
   </si>
 </sst>
 </file>
@@ -2652,8 +2661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="C62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,9 +4106,24 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>9170</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added additional error messages for #129
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538B4C69-975B-436A-91E3-3117FB366C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77149598-063D-4654-A86A-2FAAA993B4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="291">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1142,6 +1142,25 @@
   </si>
   <si>
     <t>Name ''{0}'' of {1} of ''{2}'' does not match to naming requirements of Java Language specification.</t>
+  </si>
+  <si>
+    <t>OPEN_API_SPEC_REFERENCE_MISSING</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports to split a model into several OpenAPI specifications. If in such a case one OpenAPI specification refers to the types of another one then a dependency between OpenAPI specs has to be defined in the model.</t>
+  </si>
+  <si>
+    <t>When working with OpenAPI specifications then all complex types that are used must belong either to the same or another OpenAPI specification.
+Please make sure that OpenAPI types only use basic types or other OpenAPI types that belong to an OpenAPI specification (same or referenced one).</t>
+  </si>
+  <si>
+    <t>ORPHANED_OPEN_API_TYPE_USED</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' of type ''{1}'' uses type ''{2}'' from OpenAPI specification ''{4}''. However in the UML model there is no dependency defined between OpenAPI specification ''{3}'' to ''{4}''. Please fix your UML model.</t>
+  </si>
+  <si>
+    <t>Property ''{0}'' of type ''{1}'' uses type ''{2}''. However ''{2}'' does not belong to any OpenAPI specification and thus can not be used.</t>
   </si>
 </sst>
 </file>
@@ -2661,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4126,14 +4145,44 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>9171</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>9172</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added messages for backward compatibility
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F939E6-5CCF-418D-BE46-BE9F95F102FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678E8B76-C10A-47A8-A981-4DDB5ADEE5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="300">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1161,6 +1161,33 @@
   <si>
     <t>When working with OpenAPI specifications then all complex types that are used must belong to an OpenAPI specification.
 Please make sure that OpenAPI types only use basic types or other OpenAPI types that belong to an OpenAPI specification (same or referenced one).</t>
+  </si>
+  <si>
+    <t>BACKWARD_COMPATIBILITY_ONLY_APPLICABLE_FOR_PROPERTIES</t>
+  </si>
+  <si>
+    <t>SUCCESSOR_DOES_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>JEAF Generator support developers with special code generation for backward compatibility for Java properties. Therefor it is possible to define the successor of an already existing property. The name of the successor must match to a real property of the same class.</t>
+  </si>
+  <si>
+    <t>Properties ''generateBackwardCompatibility'' and ''successorName'' must only be set if stereotype «JEAFDeprecated» is applied on a property. Please fix your UML model.</t>
+  </si>
+  <si>
+    <t>JEAF Generator support developers with special code generation for backward compatibility for Java properties. Due to that tagged value ''generateBackwardCompatibility'' and ''successorName'' of stereotype «JEAFDeprecated» can only be used for properties.</t>
+  </si>
+  <si>
+    <t>SUCCESSOR_NOT_SET</t>
+  </si>
+  <si>
+    <t>JEAF Generator support developers with special code generation for backward compatibility for Java properties. Therefor it is possible to define the successor of an already existing property. The name of the successor must be set.</t>
+  </si>
+  <si>
+    <t>Successor name for property ''{0}'' is not set in class ''{1}'' even though it is required for code generation of backward compatible Java code.</t>
+  </si>
+  <si>
+    <t>Successor property with name ''{0}'' does not exist in class ''{1}'' nor any of ist parent classes. Please check the name of the successor property in tag ''successorName''. Available properties: {2}</t>
   </si>
 </sst>
 </file>
@@ -2680,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,19 +4212,64 @@
         <v>288</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>9173</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>9174</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>9175</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved description of error message
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1318E18A-ECED-40F7-8C78-04DC998DF051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262ADD9-9351-4AD0-AF73-F076506268F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -1156,9 +1156,6 @@
     <t>Property ''{0}'' of type ''{1}'' uses type ''{2}''. However ''{2}'' does not belong to any OpenAPI specification and thus can not be used.</t>
   </si>
   <si>
-    <t>JEAF Generator supports to split a model into several OpenAPI specifications. If in such a case one OpenAPI specification refers to the types of another one, then a dependency between OpenAPI specs has to be defined in the UML model.</t>
-  </si>
-  <si>
     <t>When working with OpenAPI specifications then all complex types that are used must belong to an OpenAPI specification.
 Please make sure that OpenAPI types only use basic types or other OpenAPI types that belong to an OpenAPI specification (same or referenced one).</t>
   </si>
@@ -1197,6 +1194,10 @@
   </si>
   <si>
     <t>JEAF Generator supports to generate NotNull / NotEmpty annotations based on the UML model information for properties and parameters. However, in Java there is no really default which annotatrion to use. So, JEAF Generator explicitly expects that the name of the annotation that should be used is defined in the Maven configuration.</t>
+  </si>
+  <si>
+    <t>JEAF Generator supports to split a model into several OpenAPI specifications. If in such a case one OpenAPI specification refers to the types of another one, then a dependency between OpenAPI specs has to be defined in the UML model.
+If you want you can disable this check using configuration parameter `disableOpenAPIDependencyChecks`. However, please be aware that not checking dependencies might lead to inconsistent or incorrect OpenAPI specifications.</t>
   </si>
 </sst>
 </file>
@@ -1852,13 +1853,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="2" max="2" width="53.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1923,18 +1924,18 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.73046875" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.73046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.3984375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>9000</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>9001</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>9002</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>9003</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>9004</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>9005</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>9006</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>9007</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9008</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9009</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>9010</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>9011</v>
       </c>
@@ -2203,7 +2204,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>9012</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>9013</v>
       </c>
@@ -2243,432 +2244,432 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>9014</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>9015</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>9016</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>9017</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>9018</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>9019</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>9020</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>9021</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>9022</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>9023</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>9024</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>9025</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>9026</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>9027</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>9028</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>9029</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>9030</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>9031</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>9032</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>9033</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>9034</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>9035</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>9036</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>9037</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>9038</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>9039</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>9040</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>9041</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>9042</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>9043</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>9044</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>9045</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>9046</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>9047</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>9048</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>9049</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>9050</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>9051</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>9052</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>9053</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>9054</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>9055</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>9056</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>9057</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>9058</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>9059</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>9060</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>9061</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>9062</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>9063</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>9064</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>9065</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>9066</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>9067</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>9068</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>9069</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>9070</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>9071</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>9072</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>9073</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>9074</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>9075</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>9076</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>9077</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>9078</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>9079</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>9080</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>9081</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>9082</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>9083</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>9084</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>9085</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>9086</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>9087</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>9088</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>9089</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>9090</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>9091</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>9092</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>9093</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>9094</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>9095</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>9096</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>9097</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>9098</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>9099</v>
       </c>
@@ -2717,22 +2718,22 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.73046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.3984375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2761,7 +2762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>9100</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>9101</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>9102</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>9103</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>9104</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>9105</v>
       </c>
@@ -2881,7 +2882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>9106</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>9107</v>
       </c>
@@ -2921,7 +2922,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9108</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9109</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>9110</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>9111</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>9112</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>9113</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>9114</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>9115</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>9116</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>9117</v>
       </c>
@@ -3121,7 +3122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>9118</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>9119</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>9120</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>9121</v>
       </c>
@@ -3201,7 +3202,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>9122</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>9123</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>9124</v>
       </c>
@@ -3261,7 +3262,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>9125</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>9126</v>
       </c>
@@ -3301,7 +3302,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>9127</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>9128</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>9129</v>
       </c>
@@ -3361,7 +3362,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>9130</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>9131</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>9132</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>9133</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>9134</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>9135</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>9136</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>9137</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>9138</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>9139</v>
       </c>
@@ -3561,7 +3562,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>9140</v>
       </c>
@@ -3581,7 +3582,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>9141</v>
       </c>
@@ -3601,7 +3602,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>9142</v>
       </c>
@@ -3621,7 +3622,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>9143</v>
       </c>
@@ -3641,7 +3642,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>9144</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>9145</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>9146</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>9147</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>9148</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>9149</v>
       </c>
@@ -3761,7 +3762,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>9150</v>
       </c>
@@ -3781,7 +3782,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>9151</v>
       </c>
@@ -3801,7 +3802,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>9152</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>9153</v>
       </c>
@@ -3841,7 +3842,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>9154</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>9155</v>
       </c>
@@ -3881,7 +3882,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>9156</v>
       </c>
@@ -3901,7 +3902,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>9157</v>
       </c>
@@ -3921,7 +3922,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>9158</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>9159</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>9160</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>9161</v>
       </c>
@@ -4001,7 +4002,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>9162</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>9163</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>9164</v>
       </c>
@@ -4061,7 +4062,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>9165</v>
       </c>
@@ -4081,7 +4082,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>9166</v>
       </c>
@@ -4101,7 +4102,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>9167</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>9168</v>
       </c>
@@ -4141,7 +4142,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>9169</v>
       </c>
@@ -4161,7 +4162,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>9170</v>
       </c>
@@ -4181,7 +4182,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>9171</v>
       </c>
@@ -4195,13 +4196,13 @@
         <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>9172</v>
       </c>
@@ -4215,18 +4216,18 @@
         <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>9173</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>12</v>
@@ -4235,18 +4236,18 @@
         <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>9174</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>12</v>
@@ -4255,163 +4256,163 @@
         <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>9175</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>9176</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>9177</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>9178</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>9179</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>9180</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>9181</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>9182</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>9183</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>9184</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>9185</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>9186</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>9187</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>9188</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>9189</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>9190</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>9191</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>9192</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>9193</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>9194</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>9195</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>9196</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>9197</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>9198</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>9199</v>
       </c>
@@ -4463,18 +4464,18 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.73046875" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.73046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.3984375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4503,7 +4504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>20000</v>
       </c>
@@ -4577,12 +4578,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4593,7 +4594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4623,17 +4624,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added error code 9177
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\JEAF\jeaf-generator-messages\jeaf-generator-messages\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tls/git/jeaf-generator-messages/jeaf-generator-messages/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129EA081-6D38-49DC-848D-43CC469E5159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F198B539-88EC-6D42-9D6E-E24011569FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="20880" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="34080" windowHeight="27040" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="306">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1198,6 +1198,15 @@
   </si>
   <si>
     <t>Property ''{0}'' in your UML model makes use of soft links with custom generic types. Please make us of Maven Plugin configuration parameter ''javaGenericSoftLinkType'' / ''openAPIGenericSoftLinkType''.</t>
+  </si>
+  <si>
+    <t>PARAMETER_WITHOUT_TYPE</t>
+  </si>
+  <si>
+    <t>When modeling parameters of methods in UML it is important that they also have a type. If a type is not defined then code generation is not possible.</t>
+  </si>
+  <si>
+    <t>Parameter ''{0}'' of method ''{1}'' has no type. Please define a type for every parameter in the UML model.</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1269,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
@@ -1551,9 +1560,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1591,7 +1600,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1697,7 +1706,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1853,13 +1862,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1875,7 +1884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1899,7 +1908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1924,18 +1933,18 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +1973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>9000</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9001</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>9002</v>
       </c>
@@ -2024,7 +2033,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9003</v>
       </c>
@@ -2044,7 +2053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>9004</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>9005</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>9006</v>
       </c>
@@ -2104,7 +2113,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9007</v>
       </c>
@@ -2124,7 +2133,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9008</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9009</v>
       </c>
@@ -2164,7 +2173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9010</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9011</v>
       </c>
@@ -2204,7 +2213,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>9012</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9013</v>
       </c>
@@ -2244,432 +2253,432 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>9014</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>9015</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9016</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>9017</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>9018</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>9019</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>9020</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>9021</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9022</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>9023</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>9024</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>9025</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>9026</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>9027</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>9028</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>9029</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>9030</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>9031</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>9032</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>9033</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>9034</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>9035</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>9036</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>9037</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>9038</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>9039</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>9040</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>9041</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>9042</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>9043</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>9044</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>9045</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>9046</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>9047</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>9048</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>9049</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>9050</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>9051</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>9052</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>9053</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>9054</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>9055</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>9056</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>9057</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>9058</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>9059</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>9060</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>9061</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>9062</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>9063</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>9064</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>9065</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>9066</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>9067</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>9068</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>9069</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>9070</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>9071</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>9072</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>9073</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>9074</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>9075</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>9076</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>9077</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>9078</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>9079</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>9080</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>9081</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>9082</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>9083</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>9084</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>9085</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>9086</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9087</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>9088</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>9089</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>9090</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>9091</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>9092</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>9093</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>9094</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>9095</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>9096</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>9097</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>9098</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>9099</v>
       </c>
@@ -2717,23 +2726,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2762,7 +2771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>9100</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9101</v>
       </c>
@@ -2802,7 +2811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>9102</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9103</v>
       </c>
@@ -2842,7 +2851,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>9104</v>
       </c>
@@ -2862,7 +2871,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>9105</v>
       </c>
@@ -2882,7 +2891,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>9106</v>
       </c>
@@ -2902,7 +2911,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9107</v>
       </c>
@@ -2922,7 +2931,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9108</v>
       </c>
@@ -2942,7 +2951,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9109</v>
       </c>
@@ -2962,7 +2971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9110</v>
       </c>
@@ -2982,7 +2991,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9111</v>
       </c>
@@ -3002,7 +3011,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>9112</v>
       </c>
@@ -3022,7 +3031,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9113</v>
       </c>
@@ -3042,7 +3051,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>9114</v>
       </c>
@@ -3062,7 +3071,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>9115</v>
       </c>
@@ -3082,7 +3091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9116</v>
       </c>
@@ -3102,7 +3111,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>9117</v>
       </c>
@@ -3122,7 +3131,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>9118</v>
       </c>
@@ -3142,7 +3151,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>9119</v>
       </c>
@@ -3162,7 +3171,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>9120</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>9121</v>
       </c>
@@ -3202,7 +3211,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9122</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>9123</v>
       </c>
@@ -3242,7 +3251,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>9124</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>9125</v>
       </c>
@@ -3282,7 +3291,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>9126</v>
       </c>
@@ -3302,7 +3311,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>9127</v>
       </c>
@@ -3322,7 +3331,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>9128</v>
       </c>
@@ -3342,7 +3351,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>9129</v>
       </c>
@@ -3362,7 +3371,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>9130</v>
       </c>
@@ -3382,7 +3391,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>9131</v>
       </c>
@@ -3402,7 +3411,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>9132</v>
       </c>
@@ -3422,7 +3431,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>9133</v>
       </c>
@@ -3442,7 +3451,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>9134</v>
       </c>
@@ -3462,7 +3471,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>9135</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>9136</v>
       </c>
@@ -3502,7 +3511,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>9137</v>
       </c>
@@ -3522,7 +3531,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>9138</v>
       </c>
@@ -3542,7 +3551,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>9139</v>
       </c>
@@ -3562,7 +3571,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>9140</v>
       </c>
@@ -3582,7 +3591,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>9141</v>
       </c>
@@ -3602,7 +3611,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>9142</v>
       </c>
@@ -3622,7 +3631,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>9143</v>
       </c>
@@ -3642,7 +3651,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>9144</v>
       </c>
@@ -3662,7 +3671,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>9145</v>
       </c>
@@ -3682,7 +3691,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>9146</v>
       </c>
@@ -3702,7 +3711,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>9147</v>
       </c>
@@ -3722,7 +3731,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>9148</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>9149</v>
       </c>
@@ -3762,7 +3771,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>9150</v>
       </c>
@@ -3782,7 +3791,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>9151</v>
       </c>
@@ -3802,7 +3811,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>9152</v>
       </c>
@@ -3822,7 +3831,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>9153</v>
       </c>
@@ -3842,7 +3851,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="208" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>9154</v>
       </c>
@@ -3862,7 +3871,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>9155</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>9156</v>
       </c>
@@ -3902,7 +3911,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>9157</v>
       </c>
@@ -3922,7 +3931,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>9158</v>
       </c>
@@ -3942,7 +3951,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>9159</v>
       </c>
@@ -3962,7 +3971,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>9160</v>
       </c>
@@ -3982,7 +3991,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>9161</v>
       </c>
@@ -4002,7 +4011,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>9162</v>
       </c>
@@ -4022,7 +4031,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>9163</v>
       </c>
@@ -4042,7 +4051,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>9164</v>
       </c>
@@ -4062,7 +4071,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>9165</v>
       </c>
@@ -4082,7 +4091,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>9166</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>9167</v>
       </c>
@@ -4122,7 +4131,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>9168</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>9169</v>
       </c>
@@ -4162,7 +4171,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>9170</v>
       </c>
@@ -4182,7 +4191,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>9171</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>9172</v>
       </c>
@@ -4222,7 +4231,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>9173</v>
       </c>
@@ -4242,7 +4251,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>9174</v>
       </c>
@@ -4262,7 +4271,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>9175</v>
       </c>
@@ -4282,7 +4291,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>9176</v>
       </c>
@@ -4302,117 +4311,132 @@
         <v>297</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>9177</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>9178</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>9179</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>9180</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>9181</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>9182</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>9183</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>9184</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>9185</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>9186</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9187</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>9188</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>9189</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>9190</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>9191</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>9192</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>9193</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>9194</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>9195</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>9196</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>9197</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>9198</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>9199</v>
       </c>
@@ -4442,7 +4466,7 @@
           <x14:formula1>
             <xm:f>'Predefined-Values'!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E45 D2:D101</xm:sqref>
+          <xm:sqref>E3:E45 D2:D101 E79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00450C44-2AB6-4CEB-9EFF-8550DB68F674}">
           <x14:formula1>
@@ -4464,18 +4488,18 @@
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="60.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="60.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4504,7 +4528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>20000</v>
       </c>
@@ -4578,12 +4602,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4594,7 +4618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4605,7 +4629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4616,7 +4640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4624,17 +4648,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added error message for broken template binding
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tls/git/jeaf-generator-messages/jeaf-generator-messages/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillmann.schall/Projects/JEAF/jeaf-generator-messages/jeaf-generator-messages/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F198B539-88EC-6D42-9D6E-E24011569FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF59945-20FC-C841-8F51-EEA4532C2CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="520" windowWidth="34080" windowHeight="27040" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="1200" yWindow="520" windowWidth="25260" windowHeight="28260" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Message-Data-Template" sheetId="2" r:id="rId4"/>
     <sheet name="Predefined-Values" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="309">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1114,9 +1114,6 @@
     <t>TOO_MANY_TEMPLATE_BINDINGS</t>
   </si>
   <si>
-    <t>Class ''{0}'' has more than one template bindung in UML model.</t>
-  </si>
-  <si>
     <t>MANDATORY_ENUM_PROPERTIES_NOT_SET</t>
   </si>
   <si>
@@ -1207,6 +1204,18 @@
   </si>
   <si>
     <t>Parameter ''{0}'' of method ''{1}'' has no type. Please define a type for every parameter in the UML model.</t>
+  </si>
+  <si>
+    <t>BROKEN_TEMPLATE_BINDING</t>
+  </si>
+  <si>
+    <t>Class ''{0}'' has more than one template binding in UML model.</t>
+  </si>
+  <si>
+    <t>Template binding of class ''{0}'' is broken. There is no concrete type mapping defined. Please make sure that for every template parameter substitution there also is a actual type defined in the UML model.</t>
+  </si>
+  <si>
+    <t>JEAF Generator detected that there is a class with a broken template binding. Please make sure that for every template parameter substitution there also is a actual type defined in the UML model.</t>
   </si>
 </sst>
 </file>
@@ -2726,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3948,7 +3957,7 @@
         <v>244</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -4125,7 +4134,7 @@
         <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>273</v>
@@ -4145,10 +4154,10 @@
         <v>12</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -4156,19 +4165,19 @@
         <v>9169</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4176,19 +4185,19 @@
         <v>9170</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="128" x14ac:dyDescent="0.2">
@@ -4196,7 +4205,7 @@
         <v>9171</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>12</v>
@@ -4205,10 +4214,10 @@
         <v>12</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4216,7 +4225,7 @@
         <v>9172</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>12</v>
@@ -4225,10 +4234,10 @@
         <v>12</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4236,7 +4245,7 @@
         <v>9173</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>12</v>
@@ -4245,10 +4254,10 @@
         <v>12</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4256,7 +4265,7 @@
         <v>9174</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>12</v>
@@ -4265,10 +4274,10 @@
         <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4276,19 +4285,19 @@
         <v>9175</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -4296,19 +4305,19 @@
         <v>9176</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4316,24 +4325,39 @@
         <v>9177</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="1" t="s">
+      <c r="G79" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>9178</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated error messages for #8
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillmann.schall/Projects/JEAF/jeaf-generator-messages/jeaf-generator-messages/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF59945-20FC-C841-8F51-EEA4532C2CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C865B596-2E03-5D43-BDD1-8069BD499654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="520" windowWidth="25260" windowHeight="28260" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
+    <workbookView xWindow="1240" yWindow="600" windowWidth="25260" windowHeight="28200" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Info" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="312">
   <si>
     <t>Class-Info</t>
   </si>
@@ -1216,6 +1216,15 @@
   </si>
   <si>
     <t>JEAF Generator detected that there is a class with a broken template binding. Please make sure that for every template parameter substitution there also is a actual type defined in the UML model.</t>
+  </si>
+  <si>
+    <t>PROPERTY_WITH_OPTIONAL_PRIMITIVE</t>
+  </si>
+  <si>
+    <t>Class ''{0}'' has optional property ''{1}'' that uses a primitive type. This is not supported by Java.</t>
+  </si>
+  <si>
+    <t>JEAF Generator detected that there is an optional primitive property without explicit default value in a class. As this is not supported in Java it does not make sense for classes with stereotype  «POJO» or «ServiceObject»</t>
   </si>
 </sst>
 </file>
@@ -2735,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0997E48D-32AB-46C6-AE66-3A9CF4824DEA}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="C70" zoomScale="130" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4360,82 +4369,97 @@
         <v>307</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>9179</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>9180</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>9181</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>9182</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>9183</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>9184</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>9185</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>9186</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9187</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>9188</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>9189</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>9190</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>9191</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>9192</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>9193</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>9194</v>
       </c>

</xml_diff>

<commit_message>
Improved error messages for #8
</commit_message>
<xml_diff>
--- a/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
+++ b/jeaf-generator-messages/src/main/resources/JEAFGeneratorMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillmann.schall/Projects/JEAF/jeaf-generator-messages/jeaf-generator-messages/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E390722-4B04-CE4A-93D2-EB0BE9511994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362955EA-C81A-0D41-9294-4B65258ED4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="600" windowWidth="25260" windowHeight="28200" activeTab="2" xr2:uid="{ADB42BFB-6EC0-410A-8CB1-9C298A092AA4}"/>
   </bookViews>
@@ -1232,10 +1232,10 @@
 This check was excplitily enabled in your Maven configuration using configuration parameter "enforceExplicitDefaultValueForOptionalPrimitives".</t>
   </si>
   <si>
-    <t>Operation ''{0}'' has optional parameter ''{1}'' that uses a primitive type. Due to an explicitly enabled check in your Maven configuration it is required that there is an explicit default value for all optional primitive parameters.</t>
-  </si>
-  <si>
     <t>Class ''{0}'' has optional property ''{1}'' that uses a primitive type. Due to an explicitly enabled check in your Maven configuration it is required that there is an explicit default value for all optional primitive properties.</t>
+  </si>
+  <si>
+    <t>Operation ''{0}(…)'' has optional parameter ''{1}'' that uses a primitive type. Due to an explicitly enabled check in your Maven configuration it is required that there is an explicit default value for all optional primitive parameters.</t>
   </si>
 </sst>
 </file>
@@ -2756,7 +2756,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C70" zoomScale="130" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4397,7 +4397,7 @@
         <v>312</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="96" x14ac:dyDescent="0.2">
@@ -4417,7 +4417,7 @@
         <v>311</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>